<commit_message>
14 May 2022 _1
14 May 2022 _1
</commit_message>
<xml_diff>
--- a/Variables/CP3_sites.xlsx
+++ b/Variables/CP3_sites.xlsx
@@ -423,85 +423,34 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>org</t>
+          <t>username</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>entity_name</t>
+          <t>password</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>cp3_url</t>
+          <t>grant_type</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tshwane</t>
+          <t>Prioritise</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>City of Tshwane Metropolitan Municipality</t>
+          <t>Password01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.tshwane.cp3.co.za/</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Johannesburg</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>City of Johannesburg Metropolitan Municipality</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://www.joburg.cp3.co.za/</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Midvaal</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Midvaal Municipality</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://www.midvaal.cp3.co.za/</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Lekwa</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Lekwa Municipality</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>https://www.lekwa.cp3.co.za/</t>
+          <t>password</t>
         </is>
       </c>
     </row>

</xml_diff>